<commit_message>
Finalize UI/UX, theme toggle, auth flow, flash handling, dashboard cleanup, and QA-ready state
</commit_message>
<xml_diff>
--- a/testcases/Project4_Complete_50_Detailed_TestCases.xlsx
+++ b/testcases/Project4_Complete_50_Detailed_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kar Har Maidan Fateh!\project_option_b\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB4F803-1CA6-4C8D-8861-0AE2BAA59052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B0F6FD-7742-45CD-A19F-39E2443CDC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18448" yWindow="-2228" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$1:$H$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="319">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -63,21 +63,7 @@
     <t>Signup</t>
   </si>
   <si>
-    <t>Valid signup</t>
-  </si>
-  <si>
     <t>App running</t>
-  </si>
-  <si>
-    <t>1. Open browser
-2. Go to http://127.0.0.1:5000/signup
-3. Enter valid username
-4. Enter valid email
-5. Enter strong password
-6. Click Sign Up</t>
-  </si>
-  <si>
-    <t>User is registered and redirected to login page</t>
   </si>
   <si>
     <t>TC_02</t>
@@ -283,9 +269,6 @@
 3. Click Login</t>
   </si>
   <si>
-    <t>Dashboard displayed</t>
-  </si>
-  <si>
     <t>TC_17</t>
   </si>
   <si>
@@ -373,9 +356,6 @@
 3. Press browser back</t>
   </si>
   <si>
-    <t>Access denied</t>
-  </si>
-  <si>
     <t>TC_24</t>
   </si>
   <si>
@@ -391,24 +371,7 @@
     <t>TC_25</t>
   </si>
   <si>
-    <t>SQL injection login</t>
-  </si>
-  <si>
-    <t>1. Enter SQL payload
-2. Login</t>
-  </si>
-  <si>
-    <t>Rejected</t>
-  </si>
-  <si>
     <t>TC_26</t>
-  </si>
-  <si>
-    <t>XSS login</t>
-  </si>
-  <si>
-    <t>1. Enter XSS payload
-2. Login</t>
   </si>
   <si>
     <t>TC_27</t>
@@ -467,17 +430,7 @@
     <t>Dashboard</t>
   </si>
   <si>
-    <t>Access after login</t>
-  </si>
-  <si>
     <t>Logged in</t>
-  </si>
-  <si>
-    <t>1. Login
-2. Observe dashboard</t>
-  </si>
-  <si>
-    <t>Dashboard loads</t>
   </si>
   <si>
     <t>TC_32</t>
@@ -526,15 +479,9 @@
     <t>TC_36</t>
   </si>
   <si>
-    <t>Logout</t>
-  </si>
-  <si>
     <t>1. Click logout</t>
   </si>
   <si>
-    <t>User logged out</t>
-  </si>
-  <si>
     <t>TC_37</t>
   </si>
   <si>
@@ -701,13 +648,491 @@
   </si>
   <si>
     <t>Correct title</t>
+  </si>
+  <si>
+    <t>Redirected to login.
+Page UI is clean, centered, responsive, and matches final dark/light theme design. Header (App name, Date, Time, Theme toggle) and Footer (QA workflow description) are visible.</t>
+  </si>
+  <si>
+    <t>Verify :
+Login card is centered.
+Email &amp; Password fields styled uniformly.
+Primary Login CTA visible.
+Signup link visible below CTA.
+Header + Footer visible.</t>
+  </si>
+  <si>
+    <t>TC_51</t>
+  </si>
+  <si>
+    <t>TC_52</t>
+  </si>
+  <si>
+    <t>Verify Login Page Loads. Page UI is clean, centered, responsive, and matches final dark/light theme design. Header (App name, Date, Time, Theme toggle) and Footer (QA workflow description) are visible.</t>
+  </si>
+  <si>
+    <t>User exists.
+User is not logged in</t>
+  </si>
+  <si>
+    <t>User is redirected to Dashboard.
+Logged-in email is displayed correctly.
+Login and Signup links become disabled.
+Logout button becomes enabled.</t>
+  </si>
+  <si>
+    <t>Access is denied.
+Dashboard link is non-functional on Login page.
+Signup link is functional.</t>
+  </si>
+  <si>
+    <t>Signup card centered.
+Email &amp; Password fields visible with placeholders.
+Sign Up CTA visible.
+Login link visible.
+Header + Footer visible.</t>
+  </si>
+  <si>
+    <t>Verify Signup Page Loads. Page UI is clean, centered, responsive, and matches final dark/light theme design. Header (App name, Date, Time, Theme toggle) and Footer (QA workflow description) are visible.</t>
+  </si>
+  <si>
+    <t>1. Open browser
+2. Go to http://127.0.0.1:5000/signup</t>
+  </si>
+  <si>
+    <t>Dashboard link is non-functional
+Login link is functional</t>
+  </si>
+  <si>
+    <t>Verify Signup Page Navigation Links</t>
+  </si>
+  <si>
+    <t>User account created successfully.
+User redirected to Login page.</t>
+  </si>
+  <si>
+    <t>Verify user can signup successfully with valid credentials.</t>
+  </si>
+  <si>
+    <t>Verify that signup and Login links are disabled after successful login.</t>
+  </si>
+  <si>
+    <t>1. Open browser
+2. Go to http://127.0.0.1:5000/signup
+3. Enter valid email
+4. Enter strong password
+5. Click Sign Up</t>
+  </si>
+  <si>
+    <t>1. Open browser
+2. Go to http://127.0.0.1:5000/signup
+3. Enter valid email and password
+4. Click Sign Up
+5. After signup, Click on login link.
+6. Click on Dashboard link.</t>
+  </si>
+  <si>
+    <t>1. Open browser
+2. Go to http://127.0.0.1:5000/signup
+3. Enter valid email and password
+4. Click Sign Up
+5. After signup, Click on login link.
+6. Enter credentials used for signup to login.
+7. After Login, Click on Signup link.
+8. Click on login link</t>
+  </si>
+  <si>
+    <t>After login, Signup &amp; Login links must be disabled</t>
+  </si>
+  <si>
+    <t>Verify Dashboard Loads</t>
+  </si>
+  <si>
+    <t>Dashboard header card visible.
+Logged-in user email displayed.
+Logout button visible near navigation trail.
+Stats cards displayed in grid format.</t>
+  </si>
+  <si>
+    <t>1. Login with existing user credentials.
+2. Observe dashboard</t>
+  </si>
+  <si>
+    <t>Verify Logged-in User Info</t>
+  </si>
+  <si>
+    <t>“Signed in as &lt;email&gt;” must match session user</t>
+  </si>
+  <si>
+    <t>1. Login with existing user credentials.
+2. Observe Logged-in User Info</t>
+  </si>
+  <si>
+    <t>Verify Logout Functionality</t>
+  </si>
+  <si>
+    <t>User is Logged in.</t>
+  </si>
+  <si>
+    <t>User logged out successfully.
+Redirected to Login page.
+Login &amp; Signup links re-enabled.</t>
+  </si>
+  <si>
+    <t>TC_53</t>
+  </si>
+  <si>
+    <t>TC_54</t>
+  </si>
+  <si>
+    <t>TC_55</t>
+  </si>
+  <si>
+    <t>TC_56</t>
+  </si>
+  <si>
+    <t>1. Login with existing user credentials.
+2. Observe Stats card section dashboard.</t>
+  </si>
+  <si>
+    <t>Stats displayed as cards:
+Total Users
+Active Sessions
+Signups Today
+Open Issues</t>
+  </si>
+  <si>
+    <t>Verify Stats display.</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Verify header visible on all pages</t>
+  </si>
+  <si>
+    <t>Application is running</t>
+  </si>
+  <si>
+    <t>1. Open Login page
+2. Open Signup page
+3. Open Dashboard page</t>
+  </si>
+  <si>
+    <t>Header is visible on all pages with consistent layout</t>
+  </si>
+  <si>
+    <t>Verify Date shows current system date</t>
+  </si>
+  <si>
+    <t>User is on any page</t>
+  </si>
+  <si>
+    <t>1. Observe date in header
+2. Compare with system date</t>
+  </si>
+  <si>
+    <t>Displayed date matches system date</t>
+  </si>
+  <si>
+    <t>Verify Time updates dynamically</t>
+  </si>
+  <si>
+    <t>1. Observe time in header
+2. Wait 1 minute
+3. Observe again</t>
+  </si>
+  <si>
+    <t>Time updates dynamically every second/minute</t>
+  </si>
+  <si>
+    <t>Verify Theme toggle switches Dark and Light mode</t>
+  </si>
+  <si>
+    <t>1. Click Theme toggle
+2. Observe UI colors
+3. Click toggle again</t>
+  </si>
+  <si>
+    <t>UI switches between Dark and Light themes</t>
+  </si>
+  <si>
+    <t>Verify theme persists across navigation</t>
+  </si>
+  <si>
+    <t>Theme is changed</t>
+  </si>
+  <si>
+    <t>1. Change theme
+2. Navigate to another page</t>
+  </si>
+  <si>
+    <t>Selected theme persists across pages</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Verify Login and Signup links disabled after login</t>
+  </si>
+  <si>
+    <t>User is logged in</t>
+  </si>
+  <si>
+    <t>1. Login with valid credentials
+2. Observe navigation links</t>
+  </si>
+  <si>
+    <t>Login and Signup links are disabled</t>
+  </si>
+  <si>
+    <t>Verify Logout is only active link on Dashboard</t>
+  </si>
+  <si>
+    <t>1. Navigate to Dashboard
+2. Observe navigation options</t>
+  </si>
+  <si>
+    <t>Only Logout option is active</t>
+  </si>
+  <si>
+    <t>Verify Dashboard link disabled on Login page</t>
+  </si>
+  <si>
+    <t>User is logged out</t>
+  </si>
+  <si>
+    <t>1. Open Login page
+2. Observe Dashboard link</t>
+  </si>
+  <si>
+    <t>Dashboard link is disabled</t>
+  </si>
+  <si>
+    <t>Verify Dashboard link disabled on Signup page</t>
+  </si>
+  <si>
+    <t>1. Open Signup page
+2. Observe Dashboard link</t>
+  </si>
+  <si>
+    <t>Verify Total Sessions count displayed</t>
+  </si>
+  <si>
+    <t>1. Navigate to Dashboard
+2. Locate Total Sessions section</t>
+  </si>
+  <si>
+    <t>Total Sessions count is displayed correctly</t>
+  </si>
+  <si>
+    <t>Verify 7 continents listed in User Sessions Map</t>
+  </si>
+  <si>
+    <t>1. Navigate to Dashboard
+2. Observe User Sessions Map</t>
+  </si>
+  <si>
+    <t>All 7 continents are listed</t>
+  </si>
+  <si>
+    <t>Verify continent counts and percentages aligned</t>
+  </si>
+  <si>
+    <t>1. Observe continent names
+2. Observe counts and percentages</t>
+  </si>
+  <si>
+    <t>Counts and percentages are aligned correctly</t>
+  </si>
+  <si>
+    <t>Verify Page Traffic shows 7 bars</t>
+  </si>
+  <si>
+    <t>1. Navigate to Dashboard
+2. Observe Page Traffic chart</t>
+  </si>
+  <si>
+    <t>Chart displays exactly 7 bars</t>
+  </si>
+  <si>
+    <t>Verify each traffic bar shows numeric visitor count</t>
+  </si>
+  <si>
+    <t>1. Observe each bar in Page Traffic chart</t>
+  </si>
+  <si>
+    <t>Each bar displays numeric visitor count</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Verify footer visible on all pages</t>
+  </si>
+  <si>
+    <t>Footer is visible on all pages</t>
+  </si>
+  <si>
+    <t>Verify footer text describes QA workflow</t>
+  </si>
+  <si>
+    <t>Footer is visible</t>
+  </si>
+  <si>
+    <t>1. Read footer text</t>
+  </si>
+  <si>
+    <t>Footer text correctly describes QA workflow</t>
+  </si>
+  <si>
+    <t>TC_57</t>
+  </si>
+  <si>
+    <t>TC_58</t>
+  </si>
+  <si>
+    <t>TC_59</t>
+  </si>
+  <si>
+    <t>TC_60</t>
+  </si>
+  <si>
+    <t>TC_61</t>
+  </si>
+  <si>
+    <t>TC_62</t>
+  </si>
+  <si>
+    <t>TC_63</t>
+  </si>
+  <si>
+    <t>TC_64</t>
+  </si>
+  <si>
+    <t>TC_65</t>
+  </si>
+  <si>
+    <t>TC_66</t>
+  </si>
+  <si>
+    <t>TC_67</t>
+  </si>
+  <si>
+    <t>TC_68</t>
+  </si>
+  <si>
+    <t>TC_69</t>
+  </si>
+  <si>
+    <t>TC_70</t>
+  </si>
+  <si>
+    <t>TC_71</t>
+  </si>
+  <si>
+    <t>TC_72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open http://127.0.0.1:5000/login
+</t>
+  </si>
+  <si>
+    <t>Application is running.
+A valid user already exists (e.g. test25@example.com)
+Browser: Chrome (Incognito preferred)</t>
+  </si>
+  <si>
+    <t>1. Go to: http://127.0.0.1:5000/login
+2. In Email field, enter: &lt;script&gt;alert('XSS')&lt;/script&gt;
+3. In Password field, enter a valid password:
+ValidPassword123
+4. Click Login</t>
+  </si>
+  <si>
+    <t>No alert popup appears.
+No JS executes.
+Application Either shows validation error Or login fails gracefully.
+Or sanitizes input and proceeds safely.
+Page UI remains intact.
+No script visible in page source or flash messages.</t>
+  </si>
+  <si>
+    <t>Verify that XSS payload is NOT executed on Login page when a valid user exists.
+(for Email field)</t>
+  </si>
+  <si>
+    <t>Verify that XSS payload is NOT executed on Login page when a valid user exists.
+(for Password field)</t>
+  </si>
+  <si>
+    <t>1. Go to: http://127.0.0.1:5000/login
+2. In Email field, enter a valid email address
+3. In Password field, enter : &lt;script&gt;alert('XSS')&lt;/script&gt;
+4. Click Login</t>
+  </si>
+  <si>
+    <t>If secure (likely):
+XSS payload not executed. Application safely handled malicious input.
+If vulnerable:
+Alert executed on login input. XSS vulnerability confirmed.</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Verify that SQL injection payloads do NOT bypass authentication on the Login page.</t>
+  </si>
+  <si>
+    <t>Application is running.
+A valid user exists (e.g. test25@example.com).
+Database connected (normal app state).
+Browser: Chrome (Incognito recommended).</t>
+  </si>
+  <si>
+    <t>1. Open: http://127.0.0.1:5000/login
+2. In Email field, enter: ' OR '1'='1
+3. In Password field, enter anything: test123
+4. Click Login</t>
+  </si>
+  <si>
+    <t>Secure Behavior : 
+Login is rejected.
+User is NOT authenticated.
+Error message shown (generic): “Invalid credentials”.
+No redirect to dashboard.
+No DB error shown.
+UI remains stable.</t>
+  </si>
+  <si>
+    <t>1. Open: http://127.0.0.1:5000/login
+2. In Email field, enter: test25@example.com
+3. In Password field, enter : ' OR '1'='1
+4. Click Login</t>
+  </si>
+  <si>
+    <t>PASS : SQL injection payload rejected. Authentication not bypassed.
+FAIL : Login bypassed using SQL injection payload. Vulnerability confirmed.</t>
+  </si>
+  <si>
+    <t>Only for FAIL conditions :
+User logs in without valid credentials.
+Redirected to dashboard.
+Sees another user’s data.
+SQL error visible (e.g. syntax error, stack trace).</t>
+  </si>
+  <si>
+    <t>TC_73</t>
+  </si>
+  <si>
+    <t>TC_74</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,6 +1144,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1054,25 +1485,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.375" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.375" style="1"/>
-    <col min="4" max="4" width="27.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="30.375" style="1"/>
+    <col min="1" max="1" width="13.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="39" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.375" style="1"/>
     <col min="8" max="8" width="14.625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="30.375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1097,8 +1530,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="91.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1106,1000 +1542,1492 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="76.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="103.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="78.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="103.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="47.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="78.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="54.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="47.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="44.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="54.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="44.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="91.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="1" t="s">
+    <row r="23" spans="1:9" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="F23" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="1" t="s">
+    </row>
+    <row r="25" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="1" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="D26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="1" t="s">
+    <row r="27" spans="1:9" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="1" t="s">
+    <row r="28" spans="1:9" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="F28" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="1" t="s">
+    </row>
+    <row r="30" spans="1:9" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="B30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="B33" s="1" t="s">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>136</v>
+        <v>306</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>132</v>
+        <v>302</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>137</v>
+        <v>307</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>128</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B40" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="B41" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>168</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>172</v>
+        <v>127</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>176</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>221</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>184</v>
+        <v>222</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>186</v>
+        <v>139</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>187</v>
+        <v>140</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>190</v>
+        <v>143</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>192</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>194</v>
+        <v>147</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>195</v>
+        <v>148</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>196</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>198</v>
+        <v>151</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>200</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>202</v>
+        <v>156</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>203</v>
+        <v>157</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>208</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>